<commit_message>
udpate block diagrams for asic
</commit_message>
<xml_diff>
--- a/info/isa.xlsx
+++ b/info/isa.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andy1\coding\softcore_cpu\info\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andy1\coding\soft_cpu_8b\info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBF70284-F689-4E11-A676-AFB0380F758B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DBE6474-D9FD-4113-B0E5-1D7A31A9E345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{98C86FC5-E3AF-4C18-AB47-819EFB7CF919}"/>
   </bookViews>
   <sheets>
-    <sheet name="control signal decode" sheetId="4" r:id="rId1"/>
-    <sheet name="ISA" sheetId="1" r:id="rId2"/>
-    <sheet name="presudo instructions" sheetId="2" r:id="rId3"/>
+    <sheet name="asic control signal decode" sheetId="6" r:id="rId1"/>
+    <sheet name="fpga control signal decode" sheetId="4" r:id="rId2"/>
+    <sheet name="ISA" sheetId="1" r:id="rId3"/>
+    <sheet name="presudo instructions" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="174">
   <si>
     <t>comments</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -671,6 +672,12 @@
   </si>
   <si>
     <t>rf_write_sel : alu_out 0 / dmem_out 1</t>
+  </si>
+  <si>
+    <t>reg_b_write_en</t>
+  </si>
+  <si>
+    <t>reg_b_read_en</t>
   </si>
 </sst>
 </file>
@@ -977,9 +984,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1017,7 +1024,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1123,7 +1130,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1265,17 +1272,1174 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90A56920-B11D-4893-828B-9E074D852012}">
+  <dimension ref="A1:R26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K29" sqref="K29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" customWidth="1"/>
+    <col min="7" max="9" width="14.33203125" customWidth="1"/>
+    <col min="10" max="10" width="26.33203125" customWidth="1"/>
+    <col min="11" max="11" width="64.21875" customWidth="1"/>
+    <col min="12" max="13" width="29" customWidth="1"/>
+    <col min="14" max="14" width="22.33203125" customWidth="1"/>
+    <col min="15" max="15" width="27.44140625" customWidth="1"/>
+    <col min="16" max="16" width="25.44140625" customWidth="1"/>
+    <col min="17" max="17" width="38" customWidth="1"/>
+    <col min="18" max="18" width="15.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18">
+      <c r="A1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="L1" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="M1" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="N1" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="O1" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="P1" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="Q1" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="R1" s="19" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="13">
+        <v>0</v>
+      </c>
+      <c r="C2" s="13">
+        <v>0</v>
+      </c>
+      <c r="D2" s="13">
+        <v>0</v>
+      </c>
+      <c r="E2" s="13">
+        <v>0</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="L2" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14">
+        <v>1</v>
+      </c>
+      <c r="O2" s="14">
+        <v>0</v>
+      </c>
+      <c r="P2" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="14">
+        <v>0</v>
+      </c>
+      <c r="R2" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="A3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="13">
+        <v>0</v>
+      </c>
+      <c r="C3" s="13">
+        <v>0</v>
+      </c>
+      <c r="D3" s="13">
+        <v>0</v>
+      </c>
+      <c r="E3" s="13">
+        <v>1</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K3" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="L3" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14">
+        <v>1</v>
+      </c>
+      <c r="O3" s="14">
+        <v>0</v>
+      </c>
+      <c r="P3" s="14">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="14">
+        <v>0</v>
+      </c>
+      <c r="R3" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="A4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="13">
+        <v>0</v>
+      </c>
+      <c r="C4" s="13">
+        <v>0</v>
+      </c>
+      <c r="D4" s="13">
+        <v>1</v>
+      </c>
+      <c r="E4" s="13">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="L4" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14">
+        <v>1</v>
+      </c>
+      <c r="O4" s="14">
+        <v>0</v>
+      </c>
+      <c r="P4" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="14">
+        <v>0</v>
+      </c>
+      <c r="R4" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="13">
+        <v>0</v>
+      </c>
+      <c r="C5" s="13">
+        <v>0</v>
+      </c>
+      <c r="D5" s="13">
+        <v>1</v>
+      </c>
+      <c r="E5" s="13">
+        <v>1</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K5" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="L5" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14">
+        <v>1</v>
+      </c>
+      <c r="O5" s="14">
+        <v>0</v>
+      </c>
+      <c r="P5" s="14">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="14">
+        <v>0</v>
+      </c>
+      <c r="R5" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="13">
+        <v>0</v>
+      </c>
+      <c r="C6" s="13">
+        <v>1</v>
+      </c>
+      <c r="D6" s="13">
+        <v>0</v>
+      </c>
+      <c r="E6" s="13">
+        <v>0</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="L6" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14">
+        <v>1</v>
+      </c>
+      <c r="O6" s="14">
+        <v>0</v>
+      </c>
+      <c r="P6" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q6" s="14">
+        <v>0</v>
+      </c>
+      <c r="R6" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="A7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="13">
+        <v>0</v>
+      </c>
+      <c r="C7" s="13">
+        <v>1</v>
+      </c>
+      <c r="D7" s="13">
+        <v>0</v>
+      </c>
+      <c r="E7" s="13">
+        <v>1</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="L7" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14">
+        <v>1</v>
+      </c>
+      <c r="O7" s="14">
+        <v>0</v>
+      </c>
+      <c r="P7" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="14">
+        <v>0</v>
+      </c>
+      <c r="R7" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="13">
+        <v>0</v>
+      </c>
+      <c r="C8" s="13">
+        <v>1</v>
+      </c>
+      <c r="D8" s="13">
+        <v>1</v>
+      </c>
+      <c r="E8" s="13">
+        <v>0</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K8" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="L8" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14">
+        <v>1</v>
+      </c>
+      <c r="O8" s="14">
+        <v>0</v>
+      </c>
+      <c r="P8" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="14">
+        <v>0</v>
+      </c>
+      <c r="R8" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="A9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="13">
+        <v>0</v>
+      </c>
+      <c r="C9" s="13">
+        <v>1</v>
+      </c>
+      <c r="D9" s="13">
+        <v>1</v>
+      </c>
+      <c r="E9" s="13">
+        <v>1</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K9" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="L9" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="M9" s="14"/>
+      <c r="N9" s="14">
+        <v>1</v>
+      </c>
+      <c r="O9" s="14">
+        <v>0</v>
+      </c>
+      <c r="P9" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="14">
+        <v>0</v>
+      </c>
+      <c r="R9" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="A10" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" s="13">
+        <v>1</v>
+      </c>
+      <c r="C10" s="13">
+        <v>0</v>
+      </c>
+      <c r="D10" s="13">
+        <v>0</v>
+      </c>
+      <c r="E10" s="13">
+        <v>0</v>
+      </c>
+      <c r="F10" s="13">
+        <v>0</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="K10" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="L10" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="M10" s="14"/>
+      <c r="N10" s="14">
+        <v>1</v>
+      </c>
+      <c r="O10" s="14">
+        <v>0</v>
+      </c>
+      <c r="P10" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q10" s="14">
+        <v>0</v>
+      </c>
+      <c r="R10" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="A11" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B11" s="13">
+        <v>1</v>
+      </c>
+      <c r="C11" s="13">
+        <v>0</v>
+      </c>
+      <c r="D11" s="13">
+        <v>0</v>
+      </c>
+      <c r="E11" s="13">
+        <v>0</v>
+      </c>
+      <c r="F11" s="13">
+        <v>1</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="K11" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="L11" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14">
+        <v>1</v>
+      </c>
+      <c r="O11" s="14">
+        <v>1</v>
+      </c>
+      <c r="P11" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q11" s="14">
+        <v>0</v>
+      </c>
+      <c r="R11" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
+      <c r="A12" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="13">
+        <v>1</v>
+      </c>
+      <c r="C12" s="13">
+        <v>0</v>
+      </c>
+      <c r="D12" s="13">
+        <v>0</v>
+      </c>
+      <c r="E12" s="13">
+        <v>1</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="K12" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="L12" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14">
+        <v>1</v>
+      </c>
+      <c r="O12" s="14">
+        <v>0</v>
+      </c>
+      <c r="P12" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q12" s="14">
+        <v>1</v>
+      </c>
+      <c r="R12" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="A13" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="13">
+        <v>1</v>
+      </c>
+      <c r="C13" s="13">
+        <v>0</v>
+      </c>
+      <c r="D13" s="13">
+        <v>1</v>
+      </c>
+      <c r="E13" s="13">
+        <v>0</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="K13" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="L13" s="14" t="s">
+        <v>164</v>
+      </c>
+      <c r="M13" s="14"/>
+      <c r="N13" s="14">
+        <v>0</v>
+      </c>
+      <c r="O13" s="14">
+        <v>0</v>
+      </c>
+      <c r="P13" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="R13" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="A14" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="13">
+        <v>1</v>
+      </c>
+      <c r="C14" s="13">
+        <v>0</v>
+      </c>
+      <c r="D14" s="13">
+        <v>1</v>
+      </c>
+      <c r="E14" s="13">
+        <v>1</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="K14" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="L14" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="M14" s="14"/>
+      <c r="N14" s="14">
+        <v>0</v>
+      </c>
+      <c r="O14" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="P14" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="R14" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="A15" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B15" s="13">
+        <v>1</v>
+      </c>
+      <c r="C15" s="13">
+        <v>1</v>
+      </c>
+      <c r="D15" s="13">
+        <v>0</v>
+      </c>
+      <c r="E15" s="13">
+        <v>0</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K15" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="L15" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14">
+        <v>0</v>
+      </c>
+      <c r="O15" s="14">
+        <v>1</v>
+      </c>
+      <c r="P15" s="14">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="R15" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="A16" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="13">
+        <v>1</v>
+      </c>
+      <c r="C16" s="13">
+        <v>1</v>
+      </c>
+      <c r="D16" s="13">
+        <v>0</v>
+      </c>
+      <c r="E16" s="13">
+        <v>1</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="K16" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="L16" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="M16" s="14"/>
+      <c r="N16" s="14">
+        <v>0</v>
+      </c>
+      <c r="O16" s="14">
+        <v>1</v>
+      </c>
+      <c r="P16" s="14">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="R16" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18">
+      <c r="A17" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B17" s="13">
+        <v>1</v>
+      </c>
+      <c r="C17" s="13">
+        <v>1</v>
+      </c>
+      <c r="D17" s="13">
+        <v>1</v>
+      </c>
+      <c r="E17" s="13">
+        <v>0</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="K17" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="L17" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="M17" s="14"/>
+      <c r="N17" s="14">
+        <v>0</v>
+      </c>
+      <c r="O17" s="14">
+        <v>1</v>
+      </c>
+      <c r="P17" s="14">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="R17" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18">
+      <c r="A18" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="13">
+        <v>1</v>
+      </c>
+      <c r="C18" s="13">
+        <v>1</v>
+      </c>
+      <c r="D18" s="13">
+        <v>1</v>
+      </c>
+      <c r="E18" s="13">
+        <v>1</v>
+      </c>
+      <c r="F18" s="13">
+        <v>0</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K18" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="L18" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="M18" s="14"/>
+      <c r="N18" s="14">
+        <v>0</v>
+      </c>
+      <c r="O18" s="14">
+        <v>1</v>
+      </c>
+      <c r="P18" s="14">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="R18" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18">
+      <c r="A19" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="13">
+        <v>1</v>
+      </c>
+      <c r="C19" s="13">
+        <v>1</v>
+      </c>
+      <c r="D19" s="13">
+        <v>1</v>
+      </c>
+      <c r="E19" s="13">
+        <v>1</v>
+      </c>
+      <c r="F19" s="13">
+        <v>1</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="K19" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="L19" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="M19" s="14"/>
+      <c r="N19" s="14">
+        <v>0</v>
+      </c>
+      <c r="O19" s="14">
+        <v>1</v>
+      </c>
+      <c r="P19" s="14">
+        <v>1</v>
+      </c>
+      <c r="Q19" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="R19" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18">
+      <c r="N20" s="15"/>
+      <c r="O20" s="15"/>
+    </row>
+    <row r="22" spans="1:18">
+      <c r="A22" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="21"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="22"/>
+      <c r="L22" s="15"/>
+      <c r="M22" s="15"/>
+    </row>
+    <row r="23" spans="1:18">
+      <c r="A23" s="2">
+        <v>1</v>
+      </c>
+      <c r="B23" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="23"/>
+      <c r="L23" s="16"/>
+      <c r="M23" s="16"/>
+    </row>
+    <row r="24" spans="1:18">
+      <c r="A24" s="2">
+        <v>2</v>
+      </c>
+      <c r="B24" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="C24" s="23"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="23"/>
+      <c r="I24" s="23"/>
+      <c r="J24" s="23"/>
+      <c r="L24" s="16"/>
+      <c r="M24" s="16"/>
+    </row>
+    <row r="25" spans="1:18">
+      <c r="A25" s="2">
+        <v>3</v>
+      </c>
+      <c r="B25" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="C25" s="23"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="23"/>
+      <c r="I25" s="23"/>
+      <c r="J25" s="23"/>
+      <c r="L25" s="16"/>
+      <c r="M25" s="16"/>
+    </row>
+    <row r="26" spans="1:18">
+      <c r="A26" s="2">
+        <v>4</v>
+      </c>
+      <c r="B26" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="23"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="23"/>
+      <c r="I26" s="23"/>
+      <c r="J26" s="23"/>
+      <c r="L26" s="16"/>
+      <c r="M26" s="16"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A22:J22"/>
+    <mergeCell ref="B23:J23"/>
+    <mergeCell ref="B24:J24"/>
+    <mergeCell ref="B25:J25"/>
+    <mergeCell ref="B26:J26"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B97F70D-B131-4050-83E1-4FBF1CD85DFC}">
   <dimension ref="A1:Q26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
@@ -2402,7 +3566,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECC2C441-DEC2-4001-8CD5-3DBF91AD2891}">
   <dimension ref="A1:M26"/>
   <sheetViews>
@@ -3297,7 +4461,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9DC6A67-9716-471F-B242-870F8D2F0ED7}">
   <dimension ref="A1:D34"/>
   <sheetViews>

</xml_diff>